<commit_message>
removed xlsx cached stuff
</commit_message>
<xml_diff>
--- a/experiments/overview_testcases.xlsx
+++ b/experiments/overview_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/di35hef/Projects/qulrb/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA904106-A71D-D148-A298-B29D2913E568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261DD09F-2B9F-C146-B371-D8DB0749060C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="29100" windowHeight="18780" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_testcases" sheetId="1" r:id="rId1"/>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4030A8C0-E326-C74F-9B88-3229C854A6DA}">
   <dimension ref="A2:T48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2140,14 +2140,14 @@
         <v>128</v>
       </c>
       <c r="I39">
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J39">
         <v>384</v>
       </c>
       <c r="K39" s="3">
         <f>(MAX(C39:J39)/AVERAGE(C39:J39)-1)</f>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="I40">
         <f>$I$39</f>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J40">
         <f>$J$39</f>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="K40" s="3">
         <f t="shared" ref="K40:K48" si="15">(MAX(C40:J40)/AVERAGE(C40:J40)-1)</f>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2227,7 +2227,7 @@
       </c>
       <c r="I41">
         <f t="shared" ref="I41:I48" si="22">$I$39</f>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J41">
         <f t="shared" ref="J41:J48" si="23">$J$39</f>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="K41" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="I42">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J42">
         <f t="shared" si="23"/>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="K42" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="I43">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J43">
         <f t="shared" si="23"/>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="K43" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="I44">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J44">
         <f t="shared" si="23"/>
@@ -2367,7 +2367,7 @@
       </c>
       <c r="K44" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2403,7 +2403,7 @@
       </c>
       <c r="I45">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J45">
         <f t="shared" si="23"/>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="K45" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2447,7 +2447,7 @@
       </c>
       <c r="I46">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J46">
         <f t="shared" si="23"/>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="K46" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2491,7 +2491,7 @@
       </c>
       <c r="I47">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J47">
         <f t="shared" si="23"/>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="K47" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="I48">
         <f t="shared" si="22"/>
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="J48">
         <f t="shared" si="23"/>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="K48" s="3">
         <f t="shared" si="15"/>
-        <v>0.77777777777777768</v>
+        <v>0.93939393939393945</v>
       </c>
     </row>
   </sheetData>
@@ -2557,7 +2557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA3C89D0-797C-7546-9DE8-B0C7610FB72D}">
   <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pushed some more data and test cases
</commit_message>
<xml_diff>
--- a/experiments/overview_testcases.xlsx
+++ b/experiments/overview_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/di35hef/Projects/qulrb/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5053CF8F-19F8-F14B-A454-128DEA7FB124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFDEC99-E78B-9F42-BC1D-D8915FD9CAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24060" yWindow="2320" windowWidth="19060" windowHeight="19280" activeTab="4" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" activeTab="4" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_testcases" sheetId="1" r:id="rId1"/>
@@ -244,10 +244,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -783,7 +784,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,6 +807,8 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1163,7 +1166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4030A8C0-E326-C74F-9B88-3229C854A6DA}">
   <dimension ref="A2:T48"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -2671,7 +2674,7 @@
   <dimension ref="B3:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9:K11"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2925,7 +2928,7 @@
   <dimension ref="A3:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F36"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3619,10 +3622,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD917A54-0454-2C47-863F-C812DC78FCDB}">
-  <dimension ref="B3:G36"/>
+  <dimension ref="B3:O36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G36"/>
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3630,7 +3633,7 @@
     <col min="2" max="2" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
@@ -3650,7 +3653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
@@ -3663,10 +3666,14 @@
       <c r="E4" s="13">
         <v>1.9000000000000001E-4</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F4" s="9">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="G4" s="13">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>34</v>
       </c>
@@ -3679,10 +3686,14 @@
       <c r="E5" s="13">
         <v>1.2999999999999999E-4</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F5" s="13">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
@@ -3695,10 +3706,14 @@
       <c r="E6" s="13">
         <v>1.273E-2</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F6" s="9">
+        <v>1.6029999999999999E-2</v>
+      </c>
+      <c r="G6" s="9">
+        <v>2.1669999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
@@ -3707,8 +3722,9 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="O7" s="21"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -3718,7 +3734,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
@@ -3728,7 +3744,7 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
@@ -3748,7 +3764,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
@@ -3761,10 +3777,14 @@
       <c r="E13" s="14">
         <v>2.99343</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F13" s="9">
+        <v>3.4077299999999999</v>
+      </c>
+      <c r="G13" s="9">
+        <v>5.5578700000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
@@ -3777,10 +3797,14 @@
       <c r="E14" s="14">
         <v>2.9935900000000002</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F14" s="9">
+        <v>3.40856</v>
+      </c>
+      <c r="G14" s="9">
+        <v>5.5584499999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
@@ -3793,10 +3817,14 @@
       <c r="E15" s="14">
         <v>2.9563600000000001</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F15" s="9">
+        <v>3.3548900000000001</v>
+      </c>
+      <c r="G15" s="9">
+        <v>5.4405700000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -3859,8 +3887,12 @@
       <c r="E22" s="12">
         <v>1499</v>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="F22" s="9">
+        <v>3105</v>
+      </c>
+      <c r="G22" s="9">
+        <v>6302</v>
+      </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
@@ -3875,8 +3907,12 @@
       <c r="E23" s="12">
         <v>1501</v>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="F23" s="9">
+        <v>3098</v>
+      </c>
+      <c r="G23" s="9">
+        <v>6302</v>
+      </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
@@ -3891,8 +3927,12 @@
       <c r="E24" s="12">
         <v>350</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="F24" s="9">
+        <v>644</v>
+      </c>
+      <c r="G24" s="9">
+        <v>2353</v>
+      </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
@@ -3957,8 +3997,12 @@
       <c r="E31" s="12">
         <v>93.6875</v>
       </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="F31" s="9">
+        <v>97.03125</v>
+      </c>
+      <c r="G31" s="9">
+        <v>98.46875</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
@@ -3973,8 +4017,12 @@
       <c r="E32" s="12">
         <v>93.8125</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="F32" s="13">
+        <v>96.8125</v>
+      </c>
+      <c r="G32" s="9">
+        <v>98.46875</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -3989,8 +4037,12 @@
       <c r="E33" s="12">
         <v>21.875</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="F33" s="13">
+        <v>20.125</v>
+      </c>
+      <c r="G33" s="13">
+        <v>36.765625</v>
+      </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
@@ -4032,12 +4084,14 @@
   <dimension ref="B4:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="3" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -4073,40 +4127,88 @@
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0</v>
+      </c>
+      <c r="J5" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="C6" s="13">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="13">
+        <v>0</v>
+      </c>
+      <c r="G6" s="13">
+        <v>0</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="C7" s="13">
+        <v>0.13766</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.10249999999999999</v>
+      </c>
+      <c r="E7" s="13">
+        <v>3.3450000000000001E-2</v>
+      </c>
+      <c r="F7" s="13">
+        <v>2.5850000000000001E-2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>6.4700000000000001E-3</v>
+      </c>
+      <c r="H7" s="9">
+        <v>3.1199999999999999E-3</v>
+      </c>
+      <c r="I7" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J7" s="9">
+        <v>1.06E-3</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -4180,40 +4282,88 @@
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="C14" s="13">
+        <v>3.31372</v>
+      </c>
+      <c r="D14" s="13">
+        <v>3.3645</v>
+      </c>
+      <c r="E14" s="13">
+        <v>3.25691</v>
+      </c>
+      <c r="F14" s="13">
+        <v>3.2837299999999998</v>
+      </c>
+      <c r="G14" s="13">
+        <v>3.27285</v>
+      </c>
+      <c r="H14" s="9">
+        <v>3.2922899999999999</v>
+      </c>
+      <c r="I14" s="9">
+        <v>3.286</v>
+      </c>
+      <c r="J14" s="9">
+        <v>3.2961</v>
+      </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
+      <c r="C15" s="13">
+        <v>3.31372</v>
+      </c>
+      <c r="D15" s="13">
+        <v>3.3645</v>
+      </c>
+      <c r="E15" s="13">
+        <v>3.25691</v>
+      </c>
+      <c r="F15" s="13">
+        <v>3.2837299999999998</v>
+      </c>
+      <c r="G15" s="13">
+        <v>3.27285</v>
+      </c>
+      <c r="H15" s="9">
+        <v>3.2922899999999999</v>
+      </c>
+      <c r="I15" s="9">
+        <v>3.286</v>
+      </c>
+      <c r="J15" s="9">
+        <v>3.2961</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
+      <c r="C16" s="13">
+        <v>2.91275</v>
+      </c>
+      <c r="D16" s="13">
+        <v>3.05172</v>
+      </c>
+      <c r="E16" s="13">
+        <v>3.1514899999999999</v>
+      </c>
+      <c r="F16" s="13">
+        <v>3.2009799999999999</v>
+      </c>
+      <c r="G16" s="13">
+        <v>3.2518099999999999</v>
+      </c>
+      <c r="H16" s="9">
+        <v>3.2820499999999999</v>
+      </c>
+      <c r="I16" s="9">
+        <v>3.27616</v>
+      </c>
+      <c r="J16" s="9">
+        <v>3.2926000000000002</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
@@ -4287,79 +4437,127 @@
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
+      <c r="C23" s="20">
+        <v>56</v>
+      </c>
+      <c r="D23" s="20">
+        <v>112</v>
+      </c>
+      <c r="E23" s="20">
+        <v>224</v>
+      </c>
+      <c r="F23" s="20">
+        <v>448</v>
+      </c>
+      <c r="G23" s="20">
+        <v>896</v>
+      </c>
+      <c r="H23" s="20">
+        <v>1792</v>
+      </c>
+      <c r="I23" s="20">
+        <v>3584</v>
+      </c>
+      <c r="J23" s="20">
+        <v>7168</v>
+      </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
+      <c r="C24" s="20">
+        <v>56</v>
+      </c>
+      <c r="D24" s="20">
+        <v>112</v>
+      </c>
+      <c r="E24" s="20">
+        <v>224</v>
+      </c>
+      <c r="F24" s="20">
+        <v>448</v>
+      </c>
+      <c r="G24" s="20">
+        <v>896</v>
+      </c>
+      <c r="H24" s="20">
+        <v>1792</v>
+      </c>
+      <c r="I24" s="20">
+        <v>3584</v>
+      </c>
+      <c r="J24" s="20">
+        <v>7168</v>
+      </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
+      <c r="C25" s="20">
+        <v>11</v>
+      </c>
+      <c r="D25" s="20">
+        <v>53</v>
+      </c>
+      <c r="E25" s="20">
+        <v>43</v>
+      </c>
+      <c r="F25" s="20">
+        <v>87</v>
+      </c>
+      <c r="G25" s="20">
+        <v>196</v>
+      </c>
+      <c r="H25" s="20">
+        <v>349</v>
+      </c>
+      <c r="I25" s="20">
+        <v>696</v>
+      </c>
+      <c r="J25" s="20">
+        <v>1407</v>
+      </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" s="15" t="s">
@@ -4394,79 +4592,127 @@
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
+      <c r="C32" s="12">
+        <v>7</v>
+      </c>
+      <c r="D32" s="12">
+        <v>14</v>
+      </c>
+      <c r="E32" s="12">
+        <v>28</v>
+      </c>
+      <c r="F32" s="12">
+        <v>56</v>
+      </c>
+      <c r="G32" s="12">
+        <v>112</v>
+      </c>
+      <c r="H32" s="12">
+        <v>224</v>
+      </c>
+      <c r="I32" s="12">
+        <v>448</v>
+      </c>
+      <c r="J32" s="12">
+        <v>896</v>
+      </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="C33" s="12">
+        <v>7</v>
+      </c>
+      <c r="D33" s="12">
+        <v>14</v>
+      </c>
+      <c r="E33" s="12">
+        <v>28</v>
+      </c>
+      <c r="F33" s="12">
+        <v>56</v>
+      </c>
+      <c r="G33" s="12">
+        <v>112</v>
+      </c>
+      <c r="H33" s="12">
+        <v>224</v>
+      </c>
+      <c r="I33" s="12">
+        <v>448</v>
+      </c>
+      <c r="J33" s="12">
+        <v>896</v>
+      </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
+      <c r="C34" s="12">
+        <v>1.375</v>
+      </c>
+      <c r="D34" s="12">
+        <v>6.625</v>
+      </c>
+      <c r="E34" s="12">
+        <v>5.375</v>
+      </c>
+      <c r="F34" s="12">
+        <v>10.875</v>
+      </c>
+      <c r="G34" s="12">
+        <v>24.5</v>
+      </c>
+      <c r="H34" s="12">
+        <v>43.625</v>
+      </c>
+      <c r="I34" s="12">
+        <v>87</v>
+      </c>
+      <c r="J34" s="12">
+        <v>175.875</v>
+      </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
added use case with samoa osc simulation
</commit_message>
<xml_diff>
--- a/experiments/overview_testcases.xlsx
+++ b/experiments/overview_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/di35hef/Projects/qulrb/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFDEC99-E78B-9F42-BC1D-D8915FD9CAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C3D447-BBF2-A243-9F71-A1A99460F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20260" activeTab="4" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_testcases" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="83">
   <si>
     <t>1. Varied Imbalance Ratios</t>
   </si>
@@ -238,6 +238,54 @@
   </si>
   <si>
     <t>1024 tasks</t>
+  </si>
+  <si>
+    <t>qubo_cqm_k1</t>
+  </si>
+  <si>
+    <t>qubo_cqm_k2</t>
+  </si>
+  <si>
+    <t>2048 tasks</t>
+  </si>
+  <si>
+    <t>4. Realistic use case: Samoa - oscillating lake numerical simulation</t>
+  </si>
+  <si>
+    <t>Baseline</t>
+  </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>ProactLB</t>
+  </si>
+  <si>
+    <t>Gurobi</t>
+  </si>
+  <si>
+    <t>QUBO_CQM_K1</t>
+  </si>
+  <si>
+    <t>QUBO_CQM_K2</t>
+  </si>
+  <si>
+    <t>Num. total mig tasks</t>
+  </si>
+  <si>
+    <t>Cal_Rimb</t>
+  </si>
+  <si>
+    <t>Cal_Speedup</t>
+  </si>
+  <si>
+    <t>RealExp Speedup</t>
+  </si>
+  <si>
+    <t>RealExp Rimb</t>
   </si>
 </sst>
 </file>
@@ -248,7 +296,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -784,7 +832,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -807,8 +855,17 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1164,15 +1221,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4030A8C0-E326-C74F-9B88-3229C854A6DA}">
-  <dimension ref="A2:T48"/>
+  <dimension ref="A2:T71"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="18" max="18" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2661,6 +2722,157 @@
         <f t="shared" si="15"/>
         <v>0.77777777777777768</v>
       </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55">
+        <f>$C$54*C53</f>
+        <v>6656</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ref="D55:E55" si="24">$C$54*D53</f>
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="B57" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="13">
+        <v>4.1993999999999998</v>
+      </c>
+      <c r="C58" s="12">
+        <v>1</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="9">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="C59" s="9">
+        <v>5.1990499999999997</v>
+      </c>
+      <c r="D59" s="9">
+        <v>6447</v>
+      </c>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C60" s="9">
+        <v>5.1993799999999997</v>
+      </c>
+      <c r="D60" s="9">
+        <v>6447</v>
+      </c>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="9">
+        <v>9.4400000000000005E-3</v>
+      </c>
+      <c r="C61" s="9">
+        <v>5.15076</v>
+      </c>
+      <c r="D61" s="9">
+        <v>1568</v>
+      </c>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -2928,7 +3140,7 @@
   <dimension ref="A3:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H3" sqref="H3:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3093,30 +3305,30 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="13">
-        <v>0</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
-      <c r="F8" s="13">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="B8" s="9">
+        <v>7.4599999999999996E-3</v>
+      </c>
+      <c r="C8" s="9">
+        <v>7.8100000000000001E-3</v>
+      </c>
+      <c r="D8" s="9">
+        <v>8.0199999999999994E-3</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.13807</v>
+      </c>
+      <c r="F8" s="9">
+        <v>5.9040000000000002E-2</v>
       </c>
       <c r="H8" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>60.4</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>7.5540000000000003</v>
       </c>
       <c r="J8" s="9">
         <v>0</v>
@@ -3124,30 +3336,30 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="13">
-        <v>0</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1.3799999999999999E-3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2.7999999999999998E-4</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="F9" s="9">
+        <v>4.6999999999999999E-4</v>
       </c>
       <c r="H9" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="I9" s="12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>39.501999999999995</v>
       </c>
       <c r="J9" s="9">
         <v>0</v>
@@ -3255,42 +3467,42 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="14">
-        <v>0</v>
-      </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="D17" s="14">
-        <v>0</v>
-      </c>
-      <c r="E17" s="14">
-        <v>0</v>
-      </c>
-      <c r="F17" s="14">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1.0109300000000001</v>
+      </c>
+      <c r="C17" s="9">
+        <v>2.9411800000000001</v>
+      </c>
+      <c r="D17" s="9">
+        <v>3.6141100000000002</v>
+      </c>
+      <c r="E17" s="9">
+        <v>4.3633199999999999</v>
+      </c>
+      <c r="F17" s="9">
+        <v>4.1666699999999999</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B18" s="14">
-        <v>0</v>
+        <v>1.0170699999999999</v>
       </c>
       <c r="C18" s="14">
-        <v>0</v>
+        <v>2.9633099999999999</v>
       </c>
       <c r="D18" s="14">
-        <v>0</v>
+        <v>3.6424500000000002</v>
       </c>
       <c r="E18" s="14">
-        <v>0</v>
+        <v>4.9639800000000003</v>
       </c>
       <c r="F18" s="14">
-        <v>0</v>
+        <v>4.4105800000000004</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
@@ -3312,7 +3524,6 @@
       <c r="F21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
@@ -3338,7 +3549,6 @@
       <c r="F22" s="12">
         <v>353</v>
       </c>
-      <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
@@ -3365,7 +3575,6 @@
       <c r="F23" s="12">
         <v>353</v>
       </c>
-      <c r="L23" s="19"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
       <c r="O23" s="19"/>
@@ -3392,7 +3601,6 @@
       <c r="F24" s="12">
         <v>71</v>
       </c>
-      <c r="L24" s="19"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
       <c r="O24" s="19"/>
@@ -3419,7 +3627,6 @@
       <c r="F25" s="12">
         <v>0</v>
       </c>
-      <c r="L25" s="19"/>
       <c r="M25" s="19"/>
       <c r="N25" s="19"/>
       <c r="O25" s="19"/>
@@ -3429,22 +3636,22 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="12">
-        <v>0</v>
-      </c>
-      <c r="C26" s="12">
-        <v>0</v>
-      </c>
-      <c r="D26" s="12">
-        <v>0</v>
-      </c>
-      <c r="E26" s="12">
-        <v>0</v>
-      </c>
-      <c r="F26" s="12">
-        <v>0</v>
+        <v>67</v>
+      </c>
+      <c r="B26" s="9">
+        <v>2</v>
+      </c>
+      <c r="C26" s="9">
+        <v>73</v>
+      </c>
+      <c r="D26" s="9">
+        <v>107</v>
+      </c>
+      <c r="E26" s="9">
+        <v>49</v>
+      </c>
+      <c r="F26" s="9">
+        <v>71</v>
       </c>
       <c r="M26" s="18"/>
       <c r="N26" s="18"/>
@@ -3455,22 +3662,22 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="12">
-        <v>0</v>
-      </c>
-      <c r="C27" s="12">
-        <v>0</v>
-      </c>
-      <c r="D27" s="12">
-        <v>0</v>
-      </c>
-      <c r="E27" s="12">
-        <v>0</v>
-      </c>
-      <c r="F27" s="12">
-        <v>0</v>
+        <v>68</v>
+      </c>
+      <c r="B27" s="9">
+        <v>250</v>
+      </c>
+      <c r="C27" s="9">
+        <v>311</v>
+      </c>
+      <c r="D27" s="9">
+        <v>348</v>
+      </c>
+      <c r="E27" s="9">
+        <v>337</v>
+      </c>
+      <c r="F27" s="9">
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.2">
@@ -3575,42 +3782,42 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B35" s="12">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C35" s="12">
-        <v>0</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="D35" s="12">
-        <v>0</v>
+        <v>13.38</v>
       </c>
       <c r="E35" s="12">
-        <v>0</v>
+        <v>6.13</v>
       </c>
       <c r="F35" s="12">
-        <v>0</v>
+        <v>8.8800000000000008</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="B36" s="12">
-        <v>0</v>
+        <v>31.25</v>
       </c>
       <c r="C36" s="12">
-        <v>0</v>
+        <v>38.880000000000003</v>
       </c>
       <c r="D36" s="12">
-        <v>0</v>
+        <v>43.5</v>
       </c>
       <c r="E36" s="12">
-        <v>0</v>
+        <v>42.13</v>
       </c>
       <c r="F36" s="12">
-        <v>0</v>
+        <v>41.75</v>
       </c>
     </row>
   </sheetData>
@@ -3625,12 +3832,15 @@
   <dimension ref="B3:O36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="27.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
@@ -3672,6 +3882,9 @@
       <c r="G4" s="13">
         <v>1E-4</v>
       </c>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -3692,6 +3905,9 @@
       <c r="G5" s="13">
         <v>0</v>
       </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
@@ -3712,6 +3928,9 @@
       <c r="G6" s="9">
         <v>2.1669999999999998E-2</v>
       </c>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -3722,27 +3941,53 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="24"/>
       <c r="O7" s="21"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+        <v>67</v>
+      </c>
+      <c r="C8" s="13">
+        <v>2.5500000000000002E-4</v>
+      </c>
+      <c r="D8" s="13">
+        <v>8.3000000000000001E-4</v>
+      </c>
+      <c r="E8" s="13">
+        <v>8.4000000000000003E-4</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="24"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
+        <v>68</v>
+      </c>
+      <c r="C9" s="13">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1.1E-4</v>
+      </c>
+      <c r="E9" s="13">
+        <v>2.2000000000000001E-4</v>
+      </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
@@ -3836,21 +4081,33 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
+        <v>67</v>
+      </c>
+      <c r="C17" s="14">
+        <v>3.38558</v>
+      </c>
+      <c r="D17" s="14">
+        <v>3.2484600000000001</v>
+      </c>
+      <c r="E17" s="14">
+        <v>2.9914900000000002</v>
+      </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+        <v>68</v>
+      </c>
+      <c r="C18" s="14">
+        <v>3.3864299999999998</v>
+      </c>
+      <c r="D18" s="14">
+        <v>3.25082</v>
+      </c>
+      <c r="E18" s="14">
+        <v>2.9933200000000002</v>
+      </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
     </row>
@@ -3946,21 +4203,33 @@
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="C26" s="12">
+        <v>89</v>
+      </c>
+      <c r="D26" s="12">
+        <v>163</v>
+      </c>
+      <c r="E26" s="12">
+        <v>350</v>
+      </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="C27" s="12">
+        <v>285</v>
+      </c>
+      <c r="D27" s="12">
+        <v>681</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1482</v>
+      </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
     </row>
@@ -4056,35 +4325,48 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
+        <v>67</v>
+      </c>
+      <c r="C35" s="12">
+        <v>22.25</v>
+      </c>
+      <c r="D35" s="12">
+        <v>20.38</v>
+      </c>
+      <c r="E35" s="12">
+        <v>21.88</v>
+      </c>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="C36" s="12">
+        <v>71.25</v>
+      </c>
+      <c r="D36" s="12">
+        <v>85.13</v>
+      </c>
+      <c r="E36" s="12">
+        <v>92.63</v>
+      </c>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1138DB0C-5C7E-6243-9929-1A9F8BCE7023}">
-  <dimension ref="B4:J37"/>
+  <dimension ref="B4:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4094,7 +4376,7 @@
     <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -4122,8 +4404,11 @@
       <c r="J4" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
@@ -4151,8 +4436,11 @@
       <c r="J5" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
@@ -4180,8 +4468,11 @@
       <c r="J6" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
@@ -4209,8 +4500,11 @@
       <c r="J7" s="9">
         <v>1.06E-3</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="9">
+        <v>5.8E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
@@ -4222,10 +4516,11 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -4233,12 +4528,19 @@
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I9" s="13">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J9" s="13">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="K9" s="13">
+        <v>5.8199999999999997E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -4246,10 +4548,17 @@
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I10" s="9">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K10" s="9">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
@@ -4277,8 +4586,11 @@
       <c r="J13" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
@@ -4306,8 +4618,11 @@
       <c r="J14" s="9">
         <v>3.2961</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K14" s="9">
+        <v>3.2865099999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -4335,8 +4650,11 @@
       <c r="J15" s="9">
         <v>3.2961</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K15" s="9">
+        <v>3.2865099999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
@@ -4364,8 +4682,11 @@
       <c r="J16" s="9">
         <v>3.2926000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="13">
+        <v>3.2846000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
@@ -4377,10 +4698,11 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -4388,12 +4710,19 @@
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I18" s="9">
+        <v>3.27536</v>
+      </c>
+      <c r="J18" s="9">
+        <v>3.2942999999999998</v>
+      </c>
+      <c r="K18" s="9">
+        <v>3.26749</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -4401,10 +4730,17 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I19" s="9">
+        <v>3.28592</v>
+      </c>
+      <c r="J19" s="9">
+        <v>3.2961</v>
+      </c>
+      <c r="K19" s="9">
+        <v>3.2864900000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
         <v>49</v>
       </c>
@@ -4432,8 +4768,11 @@
       <c r="J22" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
@@ -4461,8 +4800,11 @@
       <c r="J23" s="20">
         <v>7168</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="9">
+        <v>14336</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
@@ -4490,8 +4832,11 @@
       <c r="J24" s="20">
         <v>7168</v>
       </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="9">
+        <v>14336</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
@@ -4519,8 +4864,11 @@
       <c r="J25" s="20">
         <v>1407</v>
       </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="9">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
@@ -4532,10 +4880,11 @@
       <c r="H26" s="20"/>
       <c r="I26" s="20"/>
       <c r="J26" s="20"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
@@ -4543,12 +4892,19 @@
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I27" s="20">
+        <v>696</v>
+      </c>
+      <c r="J27" s="20">
+        <v>1407</v>
+      </c>
+      <c r="K27" s="9">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C28" s="20"/>
       <c r="D28" s="20"/>
@@ -4556,10 +4912,17 @@
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I28" s="20">
+        <v>3022</v>
+      </c>
+      <c r="J28" s="20">
+        <v>6620</v>
+      </c>
+      <c r="K28" s="9">
+        <v>13937</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="15" t="s">
         <v>50</v>
       </c>
@@ -4587,8 +4950,11 @@
       <c r="J31" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
@@ -4616,8 +4982,11 @@
       <c r="J32" s="12">
         <v>896</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="9">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
@@ -4645,8 +5014,11 @@
       <c r="J33" s="12">
         <v>896</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="9">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>43</v>
       </c>
@@ -4674,8 +5046,11 @@
       <c r="J34" s="12">
         <v>175.875</v>
       </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="9">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>35</v>
       </c>
@@ -4687,10 +5062,11 @@
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
@@ -4698,12 +5074,19 @@
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
       <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="I36" s="12">
+        <v>87</v>
+      </c>
+      <c r="J36" s="12">
+        <v>175.875</v>
+      </c>
+      <c r="K36" s="9">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
@@ -4711,8 +5094,15 @@
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
+      <c r="I37" s="12">
+        <v>377.75</v>
+      </c>
+      <c r="J37" s="12">
+        <v>827.5</v>
+      </c>
+      <c r="K37" s="9">
+        <v>1746.625</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
updated results and plotting scripts
</commit_message>
<xml_diff>
--- a/experiments/overview_testcases.xlsx
+++ b/experiments/overview_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/di35hef/Projects/qulrb/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C3D447-BBF2-A243-9F71-A1A99460F1E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410CED1E-2FA3-B141-A93C-D9338497C9CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="20260" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
+    <workbookView xWindow="1740" yWindow="1340" windowWidth="32820" windowHeight="19680" xr2:uid="{812FFC38-D564-894D-9C8E-3521AA0E7095}"/>
   </bookViews>
   <sheets>
     <sheet name="overview_testcases" sheetId="1" r:id="rId1"/>
@@ -276,16 +276,16 @@
     <t>Num. total mig tasks</t>
   </si>
   <si>
-    <t>Cal_Rimb</t>
-  </si>
-  <si>
-    <t>Cal_Speedup</t>
-  </si>
-  <si>
-    <t>RealExp Speedup</t>
-  </si>
-  <si>
-    <t>RealExp Rimb</t>
+    <t>Runtime (us)</t>
+  </si>
+  <si>
+    <t>Speedup (Real Experiments)</t>
+  </si>
+  <si>
+    <t>Rimb (Calculation)</t>
+  </si>
+  <si>
+    <t>Speedup (Calculation)</t>
   </si>
 </sst>
 </file>
@@ -861,11 +861,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1223,14 +1221,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4030A8C0-E326-C74F-9B88-3229C854A6DA}">
   <dimension ref="A2:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
@@ -2752,30 +2751,22 @@
         <f>$C$54*C53</f>
         <v>6656</v>
       </c>
-      <c r="D55">
-        <f t="shared" ref="D55:E55" si="24">$C$54*D53</f>
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="B57" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E57" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="25" t="s">
+      <c r="F57" s="25" t="s">
         <v>80</v>
-      </c>
-      <c r="D57" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="E57" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F57" s="26" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -3140,7 +3131,7 @@
   <dimension ref="A3:R36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:J9"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3331,7 +3322,7 @@
         <v>7.5540000000000003</v>
       </c>
       <c r="J8" s="9">
-        <v>0</v>
+        <v>32035.4</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -3362,7 +3353,7 @@
         <v>39.501999999999995</v>
       </c>
       <c r="J9" s="9">
-        <v>0</v>
+        <v>32066.799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -3832,7 +3823,7 @@
   <dimension ref="B3:O36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="F26" sqref="F26:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3959,8 +3950,12 @@
       <c r="E8" s="13">
         <v>8.4000000000000003E-4</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="13">
+        <v>1.3699999999999999E-3</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1.1E-4</v>
+      </c>
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="24"/>
@@ -3978,8 +3973,12 @@
       <c r="E9" s="13">
         <v>2.2000000000000001E-4</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="F9" s="13">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1.1E-4</v>
+      </c>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="24"/>
@@ -4092,8 +4091,12 @@
       <c r="E17" s="14">
         <v>2.9914900000000002</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="F17" s="14">
+        <v>3.4039999999999999</v>
+      </c>
+      <c r="G17" s="14">
+        <v>5.5578000000000003</v>
+      </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
@@ -4108,8 +4111,12 @@
       <c r="E18" s="14">
         <v>2.9933200000000002</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
+      <c r="F18" s="14">
+        <v>3.4077000000000002</v>
+      </c>
+      <c r="G18" s="14">
+        <v>5.5578000000000003</v>
+      </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="15" t="s">
@@ -4135,19 +4142,19 @@
       <c r="B22" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="26">
         <v>300</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="26">
         <v>700</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="26">
         <v>1499</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="26">
         <v>3105</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="26">
         <v>6302</v>
       </c>
     </row>
@@ -4155,19 +4162,19 @@
       <c r="B23" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="26">
         <v>300</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="26">
         <v>700</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="26">
         <v>1501</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="26">
         <v>3098</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="26">
         <v>6302</v>
       </c>
     </row>
@@ -4175,19 +4182,19 @@
       <c r="B24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="26">
         <v>90</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="26">
         <v>163</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="26">
         <v>350</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="26">
         <v>644</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="26">
         <v>2353</v>
       </c>
     </row>
@@ -4195,43 +4202,51 @@
       <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="26">
         <v>89</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="26">
         <v>163</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="26">
         <v>350</v>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="F26" s="26">
+        <v>644</v>
+      </c>
+      <c r="G26" s="26">
+        <v>2353</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="12">
+      <c r="C27" s="26">
         <v>285</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="26">
         <v>681</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="26">
         <v>1482</v>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="F27" s="26">
+        <v>3053</v>
+      </c>
+      <c r="G27" s="26">
+        <v>6298</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="15" t="s">
@@ -4336,8 +4351,12 @@
       <c r="E35" s="12">
         <v>21.88</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="F35" s="12">
+        <v>20.13</v>
+      </c>
+      <c r="G35" s="12">
+        <v>36.770000000000003</v>
+      </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
@@ -4352,8 +4371,12 @@
       <c r="E36" s="12">
         <v>92.63</v>
       </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="F36" s="12">
+        <v>763.25</v>
+      </c>
+      <c r="G36" s="12">
+        <v>1574.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4363,10 +4386,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1138DB0C-5C7E-6243-9929-1A9F8BCE7023}">
-  <dimension ref="B4:K37"/>
+  <dimension ref="B4:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:K28"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4376,7 +4399,7 @@
     <col min="8" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
@@ -4408,71 +4431,71 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="G5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I5" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="J5" s="13">
-        <v>0</v>
-      </c>
-      <c r="K5" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="D6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="E6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="G6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="I6" s="13">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="J6" s="13">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K6" s="13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>43</v>
       </c>
@@ -4491,20 +4514,20 @@
       <c r="G7" s="13">
         <v>6.4700000000000001E-3</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="13">
         <v>3.1199999999999999E-3</v>
       </c>
       <c r="I7" s="13">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="13">
         <v>1.06E-3</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="13">
         <v>5.8E-4</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>35</v>
       </c>
@@ -4513,52 +4536,84 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="9"/>
+      <c r="C9" s="13">
+        <v>0.13769999999999999</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="E9" s="13">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="F9" s="13">
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="G9" s="13">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H9" s="13">
+        <v>2.7000000000000001E-3</v>
+      </c>
       <c r="I9" s="13">
-        <v>3.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="J9" s="13">
-        <v>5.5000000000000003E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="K9" s="13">
-        <v>5.8199999999999997E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="P9" s="18"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="J10" s="9">
+      <c r="C10" s="13">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="D10" s="13">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F10" s="13">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="H10" s="13">
+        <v>1E-4</v>
+      </c>
+      <c r="I10" s="13">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="K10" s="9">
+      <c r="J10" s="13">
         <v>1.0000000000000001E-5</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="13">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P10" s="18"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P11" s="18"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P12" s="18"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
@@ -4589,8 +4644,9 @@
       <c r="K13" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="P13" s="18"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
@@ -4621,8 +4677,9 @@
       <c r="K14" s="9">
         <v>3.2865099999999998</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="P14" s="18"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -4653,8 +4710,9 @@
       <c r="K15" s="9">
         <v>3.2865099999999998</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="P15" s="18"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>43</v>
       </c>
@@ -4685,8 +4743,10 @@
       <c r="K16" s="13">
         <v>3.2846000000000002</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
@@ -4699,48 +4759,86 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="9"/>
+      <c r="C18" s="13">
+        <v>2.9127000000000001</v>
+      </c>
+      <c r="D18" s="13">
+        <v>3.3605</v>
+      </c>
+      <c r="E18" s="13">
+        <v>3.1515</v>
+      </c>
+      <c r="F18" s="13">
+        <v>3.2010000000000001</v>
+      </c>
+      <c r="G18" s="13">
+        <v>3.2717999999999998</v>
+      </c>
+      <c r="H18" s="9">
+        <v>3.2835000000000001</v>
+      </c>
       <c r="I18" s="9">
-        <v>3.27536</v>
+        <v>3.2696000000000001</v>
       </c>
       <c r="J18" s="9">
         <v>3.2942999999999998</v>
       </c>
       <c r="K18" s="9">
-        <v>3.26749</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+        <v>3.2698999999999998</v>
+      </c>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="9"/>
+      <c r="C19" s="13">
+        <v>3.3041</v>
+      </c>
+      <c r="D19" s="13">
+        <v>3.363</v>
+      </c>
+      <c r="E19" s="13">
+        <v>3.2559999999999998</v>
+      </c>
+      <c r="F19" s="13">
+        <v>3.2831999999999999</v>
+      </c>
+      <c r="G19" s="13">
+        <v>3.2726000000000002</v>
+      </c>
+      <c r="H19" s="9">
+        <v>3.2921</v>
+      </c>
       <c r="I19" s="9">
-        <v>3.28592</v>
+        <v>3.2858999999999998</v>
       </c>
       <c r="J19" s="9">
-        <v>3.2961</v>
+        <v>3.2959999999999998</v>
       </c>
       <c r="K19" s="9">
-        <v>3.2864900000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+        <v>3.2865000000000002</v>
+      </c>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B22" s="15" t="s">
         <v>49</v>
       </c>
@@ -4771,8 +4869,10 @@
       <c r="K22" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
@@ -4800,11 +4900,13 @@
       <c r="J23" s="20">
         <v>7168</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="20">
         <v>14336</v>
       </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
@@ -4832,11 +4934,13 @@
       <c r="J24" s="20">
         <v>7168</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="20">
         <v>14336</v>
       </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="O24" s="24"/>
+      <c r="P24" s="24"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
@@ -4864,11 +4968,11 @@
       <c r="J25" s="20">
         <v>1407</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="20">
         <v>2800</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
@@ -4882,47 +4986,71 @@
       <c r="J26" s="20"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
+      <c r="C27" s="20">
+        <v>11</v>
+      </c>
+      <c r="D27" s="20">
+        <v>53</v>
+      </c>
+      <c r="E27" s="20">
+        <v>43</v>
+      </c>
+      <c r="F27" s="20">
+        <v>87</v>
+      </c>
+      <c r="G27" s="20">
+        <v>196</v>
+      </c>
+      <c r="H27" s="20">
+        <v>349</v>
+      </c>
       <c r="I27" s="20">
         <v>696</v>
       </c>
       <c r="J27" s="20">
         <v>1407</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="20">
         <v>2800</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
+      <c r="C28" s="20">
+        <v>54</v>
+      </c>
+      <c r="D28" s="20">
+        <v>102</v>
+      </c>
+      <c r="E28" s="20">
+        <v>211</v>
+      </c>
+      <c r="F28" s="20">
+        <v>447</v>
+      </c>
+      <c r="G28" s="20">
+        <v>855</v>
+      </c>
+      <c r="H28" s="20">
+        <v>1781</v>
+      </c>
       <c r="I28" s="20">
-        <v>3022</v>
+        <v>3501</v>
       </c>
       <c r="J28" s="20">
-        <v>6620</v>
-      </c>
-      <c r="K28" s="9">
-        <v>13937</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+        <v>7049</v>
+      </c>
+      <c r="K28" s="20">
+        <v>14248</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B31" s="15" t="s">
         <v>50</v>
       </c>
@@ -4954,35 +5082,35 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32" s="20">
         <v>7</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="20">
         <v>14</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="20">
         <v>28</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32" s="20">
         <v>56</v>
       </c>
-      <c r="G32" s="12">
+      <c r="G32" s="20">
         <v>112</v>
       </c>
-      <c r="H32" s="12">
+      <c r="H32" s="20">
         <v>224</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="20">
         <v>448</v>
       </c>
-      <c r="J32" s="12">
+      <c r="J32" s="20">
         <v>896</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="20">
         <v>1792</v>
       </c>
     </row>
@@ -4990,31 +5118,31 @@
       <c r="B33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33" s="20">
         <v>7</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="20">
         <v>14</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="20">
         <v>28</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33" s="20">
         <v>56</v>
       </c>
-      <c r="G33" s="12">
+      <c r="G33" s="20">
         <v>112</v>
       </c>
-      <c r="H33" s="12">
+      <c r="H33" s="20">
         <v>224</v>
       </c>
-      <c r="I33" s="12">
+      <c r="I33" s="20">
         <v>448</v>
       </c>
-      <c r="J33" s="12">
+      <c r="J33" s="20">
         <v>896</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33" s="20">
         <v>1792</v>
       </c>
     </row>
@@ -5022,31 +5150,31 @@
       <c r="B34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="20">
         <v>1.375</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="20">
         <v>6.625</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="20">
         <v>5.375</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34" s="20">
         <v>10.875</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="20">
         <v>24.5</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="20">
         <v>43.625</v>
       </c>
-      <c r="I34" s="12">
+      <c r="I34" s="20">
         <v>87</v>
       </c>
-      <c r="J34" s="12">
+      <c r="J34" s="20">
         <v>175.875</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="20">
         <v>350</v>
       </c>
     </row>
@@ -5054,33 +5182,45 @@
       <c r="B35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="9"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12">
+      <c r="C36" s="20">
+        <v>1.38</v>
+      </c>
+      <c r="D36" s="20">
+        <v>6.63</v>
+      </c>
+      <c r="E36" s="20">
+        <v>5.38</v>
+      </c>
+      <c r="F36" s="20">
+        <v>10.88</v>
+      </c>
+      <c r="G36" s="20">
+        <v>24.5</v>
+      </c>
+      <c r="H36" s="20">
+        <v>43.63</v>
+      </c>
+      <c r="I36" s="20">
         <v>87</v>
       </c>
-      <c r="J36" s="12">
-        <v>175.875</v>
-      </c>
-      <c r="K36" s="9">
+      <c r="J36" s="20">
+        <v>175.88</v>
+      </c>
+      <c r="K36" s="20">
         <v>350</v>
       </c>
     </row>
@@ -5088,25 +5228,38 @@
       <c r="B37" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12">
-        <v>377.75</v>
-      </c>
-      <c r="J37" s="12">
-        <v>827.5</v>
-      </c>
-      <c r="K37" s="9">
-        <v>1746.625</v>
+      <c r="C37" s="20">
+        <v>6.75</v>
+      </c>
+      <c r="D37" s="20">
+        <v>12.75</v>
+      </c>
+      <c r="E37" s="20">
+        <v>26.38</v>
+      </c>
+      <c r="F37" s="20">
+        <v>55.88</v>
+      </c>
+      <c r="G37" s="20">
+        <v>106.88</v>
+      </c>
+      <c r="H37" s="20">
+        <v>222.63</v>
+      </c>
+      <c r="I37" s="20">
+        <v>437.63</v>
+      </c>
+      <c r="J37" s="20">
+        <v>881.13</v>
+      </c>
+      <c r="K37" s="20">
+        <v>1781</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>